<commit_message>
Minor changes to MyAccount Test
</commit_message>
<xml_diff>
--- a/Data/Login.xlsx
+++ b/Data/Login.xlsx
@@ -36,7 +36,7 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>stage</t>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>